<commit_message>
perbaikan view pada master barang sesuai dengan sturktur terbaru
</commit_message>
<xml_diff>
--- a/public/Export_Report.xlsx
+++ b/public/Export_Report.xlsx
@@ -405,10 +405,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -437,14 +437,65 @@
       <c r="B4" s="2">
         <v>0</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="2">
+        <v>24</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="2">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2">
         <v>1</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E5" s="2">
         <v>7000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>24</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="2">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2">
+        <v>24</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="2">
+        <v>200000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>